<commit_message>
Added result graphs Added chapters to report Added dissertation guide
</commit_message>
<xml_diff>
--- a/report/Power Test results.xlsx
+++ b/report/Power Test results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="22980" windowHeight="9528"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="22980" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -73,6 +73,977 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-GB"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Power draw over time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Volts(V)</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>hh:mm</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0.54166666666666663</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.54861111111111105</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.55555555555555558</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5625</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.56944444444444442</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.57638888888888895</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.58333333333333337</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.59027777777777779</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.59722222222222221</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.60416666666666663</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.61111111111111105</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.61805555555555558</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.625</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.63194444444444442</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.63888888888888895</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.64583333333333337</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.65277777777777779</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.65972222222222221</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.67361111111111116</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.68055555555555547</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.6875</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.69444444444444453</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.70138888888888884</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.70833333333333337</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>5.03</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.03</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.04</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Amps(A)</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Watts(W)</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>2.1629</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.016</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9656</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9656</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9152</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.9656</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9656</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.1168</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.7639999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.9656</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.7639999999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.8144</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.9656</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.1168</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.0663999999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.9152</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.016</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.016</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.2176</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.9656</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.2176</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.3138000000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.4192</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.4695999999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.2680000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="b"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:axId val="75768960"/>
+        <c:axId val="75770496"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="75768960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="hh:mm" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="75770496"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="75770496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="75768960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-GB"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Power draw over time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Volts(V)</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>hh:mm</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0.54166666666666663</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.54861111111111105</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.55555555555555558</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5625</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.56944444444444442</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.57638888888888895</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.58333333333333337</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.59027777777777779</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.59722222222222221</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.60416666666666663</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.61111111111111105</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.61805555555555558</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.625</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.63194444444444442</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.63888888888888895</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.64583333333333337</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.65277777777777779</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.65972222222222221</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.67361111111111116</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.68055555555555547</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.6875</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.69444444444444453</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.70138888888888884</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.70833333333333337</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>5.03</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.03</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.04</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Amps(A)</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Power(W)</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>2.1629</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.016</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9656</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9656</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9152</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.9656</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9656</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.1168</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.7639999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.9656</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.7639999999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.8144</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.9656</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.1168</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.0663999999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.9152</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.016</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.016</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.2176</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.9656</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.2176</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.3138000000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.4192</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.4695999999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.2680000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="87557632"/>
+        <c:axId val="85327872"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="87557632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="hh:mm" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="85327872"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="85327872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="87557632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>171448</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>114302</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -362,11 +1333,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="T28" sqref="T28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -759,6 +1730,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -768,7 +1740,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -780,7 +1752,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>